<commit_message>
Signed-off-by: locdv <dinhvanloc25@gmail.com> thêm dialog comfirm khi remove account
</commit_message>
<xml_diff>
--- a/Datatest/Leads.xlsx
+++ b/Datatest/Leads.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="60">
   <si>
     <t>Id</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>Nhung17</t>
+  </si>
+  <si>
+    <t>Nhung18</t>
+  </si>
+  <si>
+    <t>Nhung19</t>
   </si>
 </sst>
 </file>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,6 +1513,98 @@
         <v>31</v>
       </c>
     </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" ref="D22:D23" si="4">B22&amp;"@Gmail.com"</f>
+        <v>Nhung18@Gmail.com</v>
+      </c>
+      <c r="E22">
+        <v>947948010</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" ref="M22:M23" si="5">B22&amp;C22</f>
+        <v>Nhung18Nguyen</v>
+      </c>
+      <c r="N22">
+        <v>33.78</v>
+      </c>
+      <c r="O22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="4"/>
+        <v>Nhung19@Gmail.com</v>
+      </c>
+      <c r="E23">
+        <v>947948011</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="5"/>
+        <v>Nhung19Nguyen</v>
+      </c>
+      <c r="N23">
+        <v>34.78</v>
+      </c>
+      <c r="O23" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1"/>
@@ -1528,6 +1626,8 @@
     <hyperlink ref="I19" r:id="rId17"/>
     <hyperlink ref="I20" r:id="rId18"/>
     <hyperlink ref="I21" r:id="rId19"/>
+    <hyperlink ref="I22" r:id="rId20"/>
+    <hyperlink ref="I23" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Signed-off-by: locdv <dinhvanloc25@gmail.com> add delete view and detail view for lead. detail view not have comment
</commit_message>
<xml_diff>
--- a/Datatest/Leads.xlsx
+++ b/Datatest/Leads.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="61">
   <si>
     <t>Id</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Nhung19</t>
+  </si>
+  <si>
+    <t>+84947947990</t>
   </si>
 </sst>
 </file>
@@ -239,8 +242,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +537,7 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -607,8 +611,8 @@
         <f>B2&amp;"@Gmail.com"</f>
         <v>dung@Gmail.com</v>
       </c>
-      <c r="E2">
-        <v>947947990</v>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>33</v>
@@ -653,8 +657,8 @@
         <f t="shared" ref="D3:D5" si="0">B3&amp;"@Gmail.com"</f>
         <v>thu@Gmail.com</v>
       </c>
-      <c r="E3">
-        <v>947947991</v>
+      <c r="E3" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
@@ -699,8 +703,8 @@
         <f t="shared" si="0"/>
         <v>lanh@Gmail.com</v>
       </c>
-      <c r="E4">
-        <v>947947992</v>
+      <c r="E4" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F4" t="s">
         <v>33</v>
@@ -745,8 +749,8 @@
         <f t="shared" si="0"/>
         <v>Nhung1@Gmail.com</v>
       </c>
-      <c r="E5">
-        <v>947947993</v>
+      <c r="E5" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -791,8 +795,8 @@
         <f t="shared" ref="D6:D21" si="2">B6&amp;"@Gmail.com"</f>
         <v>Nhung2@Gmail.com</v>
       </c>
-      <c r="E6">
-        <v>947947994</v>
+      <c r="E6" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -837,8 +841,8 @@
         <f t="shared" si="2"/>
         <v>Nhung3@Gmail.com</v>
       </c>
-      <c r="E7">
-        <v>947947995</v>
+      <c r="E7" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
@@ -883,8 +887,8 @@
         <f t="shared" si="2"/>
         <v>Nhung4@Gmail.com</v>
       </c>
-      <c r="E8">
-        <v>947947996</v>
+      <c r="E8" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
@@ -929,8 +933,8 @@
         <f t="shared" si="2"/>
         <v>Nhung5@Gmail.com</v>
       </c>
-      <c r="E9">
-        <v>947947997</v>
+      <c r="E9" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
@@ -975,8 +979,8 @@
         <f t="shared" si="2"/>
         <v>Nhung6@Gmail.com</v>
       </c>
-      <c r="E10">
-        <v>947947998</v>
+      <c r="E10" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
@@ -1021,8 +1025,8 @@
         <f t="shared" si="2"/>
         <v>Nhung7@Gmail.com</v>
       </c>
-      <c r="E11">
-        <v>947947999</v>
+      <c r="E11" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F11" t="s">
         <v>34</v>
@@ -1067,8 +1071,8 @@
         <f t="shared" si="2"/>
         <v>Nhung8@Gmail.com</v>
       </c>
-      <c r="E12">
-        <v>947948000</v>
+      <c r="E12" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
@@ -1113,8 +1117,8 @@
         <f t="shared" si="2"/>
         <v>Nhung9@Gmail.com</v>
       </c>
-      <c r="E13">
-        <v>947948001</v>
+      <c r="E13" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
@@ -1159,8 +1163,8 @@
         <f t="shared" si="2"/>
         <v>Nhung10@Gmail.com</v>
       </c>
-      <c r="E14">
-        <v>947948002</v>
+      <c r="E14" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F14" t="s">
         <v>34</v>
@@ -1205,8 +1209,8 @@
         <f t="shared" si="2"/>
         <v>Nhung11@Gmail.com</v>
       </c>
-      <c r="E15">
-        <v>947948003</v>
+      <c r="E15" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F15" t="s">
         <v>34</v>
@@ -1251,8 +1255,8 @@
         <f t="shared" si="2"/>
         <v>Nhung12@Gmail.com</v>
       </c>
-      <c r="E16">
-        <v>947948004</v>
+      <c r="E16" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F16" t="s">
         <v>34</v>
@@ -1297,8 +1301,8 @@
         <f t="shared" si="2"/>
         <v>Nhung13@Gmail.com</v>
       </c>
-      <c r="E17">
-        <v>947948005</v>
+      <c r="E17" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F17" t="s">
         <v>34</v>
@@ -1343,8 +1347,8 @@
         <f t="shared" si="2"/>
         <v>Nhung14@Gmail.com</v>
       </c>
-      <c r="E18">
-        <v>947948006</v>
+      <c r="E18" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F18" t="s">
         <v>34</v>
@@ -1389,8 +1393,8 @@
         <f t="shared" si="2"/>
         <v>Nhung15@Gmail.com</v>
       </c>
-      <c r="E19">
-        <v>947948007</v>
+      <c r="E19" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F19" t="s">
         <v>34</v>
@@ -1435,8 +1439,8 @@
         <f t="shared" si="2"/>
         <v>Nhung16@Gmail.com</v>
       </c>
-      <c r="E20">
-        <v>947948008</v>
+      <c r="E20" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F20" t="s">
         <v>34</v>
@@ -1481,8 +1485,8 @@
         <f t="shared" si="2"/>
         <v>Nhung17@Gmail.com</v>
       </c>
-      <c r="E21">
-        <v>947948009</v>
+      <c r="E21" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F21" t="s">
         <v>34</v>
@@ -1527,8 +1531,8 @@
         <f t="shared" ref="D22:D23" si="4">B22&amp;"@Gmail.com"</f>
         <v>Nhung18@Gmail.com</v>
       </c>
-      <c r="E22">
-        <v>947948010</v>
+      <c r="E22" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
@@ -1573,8 +1577,8 @@
         <f t="shared" si="4"/>
         <v>Nhung19@Gmail.com</v>
       </c>
-      <c r="E23">
-        <v>947948011</v>
+      <c r="E23" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="F23" t="s">
         <v>34</v>

</xml_diff>